<commit_message>
Signed-off-by: STUDENT John J. O Sullivan <John.J.OSullivan@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/My project/Assignment 1.xlsx
+++ b/My project/Assignment 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T00234079\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T00234079\Desktop\CG2024\My project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4524507A-5A07-4453-BA5A-4DC9034DDBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9207554-6558-425A-A8DB-AEFE44CCBB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,30 +534,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -725,6 +725,503 @@
         <a:xfrm>
           <a:off x="2638425" y="8001000"/>
           <a:ext cx="2181529" cy="4877481"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1038225</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1160860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31F37A53-D71B-4A7E-AB26-06FB35BEE0D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2867025" y="13525500"/>
+          <a:ext cx="1733550" cy="1160860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>5167724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B40A5E-E96E-467E-99CD-4B6E024E8BF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524125" y="15030450"/>
+          <a:ext cx="2457450" cy="5167724"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>861270</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>522941</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1352550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CED3CC35-68B4-4176-A062-CE774358091F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2690070" y="20564475"/>
+          <a:ext cx="2166746" cy="1343025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>714374</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>182375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>4972422</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3332DD3E-BC68-439B-9DB2-C7BBB30A6630}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2543174" y="22423250"/>
+          <a:ext cx="2352675" cy="4790047"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>154544</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>274008</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>758814</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>842946</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD6165FC-DED7-40F9-A081-2026C1A466D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8348654" y="13765583"/>
+          <a:ext cx="2444030" cy="568938"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>156576</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>13048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>790680</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>5162724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DDCF1DA-AEA3-4C42-85C8-DA5740C18153}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8350686" y="22194555"/>
+          <a:ext cx="2473864" cy="5149676"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>52192</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>300102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1226507</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1053220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70F77B14-E7CB-4372-B64B-CA8FDCDE9980}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1891952" y="28000890"/>
+          <a:ext cx="3679521" cy="753118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>743731</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>13048</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>587156</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>2374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C4E7BA2-3AE2-46DD-807E-4297A3F4444F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2583491" y="29462260"/>
+          <a:ext cx="2348631" cy="5195456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>52192</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1435274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1202585</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>2505206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDDF7E16-F0F3-4F77-BD80-C08B5913892D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1891952" y="36403767"/>
+          <a:ext cx="3655599" cy="1069932"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>574110</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>26096</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>613254</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>5175376</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF5E240D-21C8-40C6-91EC-F751AAE37C02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2413870" y="39404795"/>
+          <a:ext cx="2544350" cy="5149280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1060,7 +1557,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1154,16 +1651,13 @@
         <v>14</v>
       </c>
       <c r="C8" s="31">
-        <f>INT((C4/10000))-5</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D8" s="31">
-        <f>MOD(INT((C4/1000)),10)-4</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="31">
-        <f>MOD(INT((C4/100)),10)-5</f>
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -1232,11 +1726,11 @@
       </c>
       <c r="D12" s="29">
         <f>C8</f>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E12" s="29">
         <f>E8</f>
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="H12" t="s">
         <v>40</v>
@@ -1286,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1311,10 +1805,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="47"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1326,7 +1820,7 @@
     <row r="3" spans="3:13" ht="408.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
       <c r="D3" s="38"/>
-      <c r="E3" s="40"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="33"/>
       <c r="G3" s="11"/>
       <c r="H3" s="34"/>
@@ -1346,10 +1840,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="41"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1359,7 +1853,7 @@
     <row r="6" spans="3:13" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
       <c r="D6" s="38"/>
-      <c r="E6" s="40"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1379,10 +1873,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="47"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1393,7 +1887,7 @@
     <row r="9" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
       <c r="D9" s="38"/>
-      <c r="E9" s="40"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1413,16 +1907,16 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="47"/>
+      <c r="E11" s="41"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="44" t="s">
+      <c r="H11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="45"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
@@ -1430,11 +1924,11 @@
     <row r="12" spans="3:13" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
       <c r="D12" s="38"/>
-      <c r="E12" s="40"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="38"/>
-      <c r="I12" s="40"/>
+      <c r="I12" s="39"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1454,10 +1948,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="47"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1470,7 +1964,7 @@
     <row r="15" spans="3:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
       <c r="D15" s="38"/>
-      <c r="E15" s="40"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1494,10 +1988,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="47"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1510,7 +2004,7 @@
     <row r="18" spans="1:13" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="40"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1531,18 +2025,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="41" t="s">
+      <c r="E20" s="41"/>
+      <c r="F20" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="44" t="s">
+      <c r="G20" s="45"/>
+      <c r="H20" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="45"/>
+      <c r="I20" s="43"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1551,11 +2045,11 @@
     <row r="21" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
       <c r="D21" s="38"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="43"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="38"/>
-      <c r="I21" s="40"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1573,25 +2067,25 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="46" t="s">
+      <c r="D23" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="47"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="44" t="s">
+      <c r="L23" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="45"/>
+      <c r="M23" s="43"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
       <c r="D24" s="38"/>
-      <c r="E24" s="40"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -1599,7 +2093,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
       <c r="L24" s="38"/>
-      <c r="M24" s="40"/>
+      <c r="M24" s="39"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1612,10 +2106,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="45"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1627,7 +2121,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="38"/>
-      <c r="E27" s="40"/>
+      <c r="E27" s="39"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1645,15 +2139,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="45"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="46" t="s">
+      <c r="D29" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="47"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1665,10 +2159,10 @@
     </row>
     <row r="30" spans="1:13" ht="322.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="38"/>
-      <c r="B30" s="40"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="25"/>
       <c r="D30" s="38"/>
-      <c r="E30" s="40"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1686,44 +2180,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="47"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="47"/>
-      <c r="F32" s="41" t="s">
+      <c r="E32" s="41"/>
+      <c r="F32" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="46" t="s">
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="47"/>
+      <c r="M32" s="41"/>
     </row>
     <row r="33" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="48"/>
-      <c r="B33" s="39"/>
+      <c r="B33" s="46"/>
       <c r="C33" s="17"/>
       <c r="D33" s="38"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="43"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="45"/>
       <c r="L33" s="38"/>
-      <c r="M33" s="39"/>
+      <c r="M33" s="46"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1735,33 +2229,46 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E35" s="45"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" ht="213.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
       <c r="D36" s="38"/>
-      <c r="E36" s="40"/>
+      <c r="E36" s="39"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
       <c r="H38" s="38"/>
-      <c r="I38" s="39"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="91" ht="0.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="H11:I11"/>
@@ -1778,25 +2285,12 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>